<commit_message>
Añadir archivos de configuración y frontend/backend
</commit_message>
<xml_diff>
--- a/Codigo/Solicitud_datos.xlsx
+++ b/Codigo/Solicitud_datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVIER VARGAS\Desktop\WhatsApp\api-whatsapp-ts\Codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8424EF0-37B1-40ED-A94C-03C748825B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A2D321-2064-4A7E-84B1-46660E7A4D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2325" windowWidth="18900" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7485" yWindow="2595" windowWidth="18900" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Numero</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>JAVIER VARGAS</t>
-  </si>
-  <si>
-    <t>0000-0000</t>
   </si>
 </sst>
 </file>
@@ -124,27 +121,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -451,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,44 +492,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2">
-        <v>230892</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1">
-        <v>5022638</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B2 B4:B1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D2 D4:D1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>